<commit_message>
Gmail done again and correct webDriver module
</commit_message>
<xml_diff>
--- a/GoogleMail/Gmail.xlsx
+++ b/GoogleMail/Gmail.xlsx
@@ -471,12 +471,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>reediklox12345678</t>
+          <t>reedikkop123</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>reedik lox</t>
+          <t>reedik lox1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">

</xml_diff>

<commit_message>
Gmail Changes. Twitter Updates. Galxe Added
</commit_message>
<xml_diff>
--- a/GoogleMail/Gmail.xlsx
+++ b/GoogleMail/Gmail.xlsx
@@ -471,12 +471,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>reedikkop123</t>
+          <t>reedikkop123456</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>reedik lox1</t>
+          <t>reed lox</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">

</xml_diff>